<commit_message>
1.build up map_projected module in map_plot.py and link them to the current structure 2.optimize the structure and redundant code
</commit_message>
<xml_diff>
--- a/GeoChemistryPy/client/output/KMeans.xlsx
+++ b/GeoChemistryPy/client/output/KMeans.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:J110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,11 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>TTP</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>clustering result</t>
         </is>
       </c>
@@ -506,7 +511,10 @@
         <v>229.59</v>
       </c>
       <c r="I2" t="n">
-        <v>4</v>
+        <v>200.7860811985793</v>
+      </c>
+      <c r="J2" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -535,7 +543,10 @@
         <v>67.42</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>219.67328</v>
+      </c>
+      <c r="J3" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -564,6 +575,9 @@
         <v>64.22404296000001</v>
       </c>
       <c r="I4" t="n">
+        <v>146.8905782359963</v>
+      </c>
+      <c r="J4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -593,7 +607,10 @@
         <v>66.80024161</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>194.3939531826629</v>
+      </c>
+      <c r="J5" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -622,6 +639,9 @@
         <v>67.80766918</v>
       </c>
       <c r="I6" t="n">
+        <v>139.5210013481891</v>
+      </c>
+      <c r="J6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -651,7 +671,10 @@
         <v>73.58253772</v>
       </c>
       <c r="I7" t="n">
-        <v>6</v>
+        <v>141.269905274554</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -680,7 +703,10 @@
         <v>58.26097259</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>161.5074793128845</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -709,7 +735,10 @@
         <v>69.37049272</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>211.3318620951872</v>
+      </c>
+      <c r="J9" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +767,10 @@
         <v>61.1</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>171.2410063241107</v>
+      </c>
+      <c r="J10" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -767,7 +799,10 @@
         <v>62.9</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>165.0336831099196</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -796,7 +831,10 @@
         <v>64.5</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>167.4266791044776</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -825,7 +863,10 @@
         <v>66.77</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>165.2836842105263</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -854,7 +895,10 @@
         <v>78.39</v>
       </c>
       <c r="I14" t="n">
-        <v>6</v>
+        <v>175.0338963446475</v>
+      </c>
+      <c r="J14" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -883,7 +927,10 @@
         <v>50.8</v>
       </c>
       <c r="I15" t="n">
-        <v>3</v>
+        <v>154.0116095238095</v>
+      </c>
+      <c r="J15" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -912,7 +959,10 @@
         <v>60.9</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>168.4999261682243</v>
+      </c>
+      <c r="J16" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -941,7 +991,10 @@
         <v>62.83</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>150.8921410404624</v>
+      </c>
+      <c r="J17" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -970,7 +1023,10 @@
         <v>64.04000000000001</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>167.8427690763052</v>
+      </c>
+      <c r="J18" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -999,7 +1055,10 @@
         <v>58.74</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>170.2389635627531</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -1028,6 +1087,9 @@
         <v>57.35</v>
       </c>
       <c r="I20" t="n">
+        <v>141.668238277512</v>
+      </c>
+      <c r="J20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1057,7 +1119,10 @@
         <v>64.20999999999999</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>166.823125490196</v>
+      </c>
+      <c r="J21" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="22">
@@ -1086,7 +1151,10 @@
         <v>53.13</v>
       </c>
       <c r="I22" t="n">
-        <v>3</v>
+        <v>135.6634228855721</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1112,10 +1180,13 @@
         <v>0.593</v>
       </c>
       <c r="H23" t="n">
-        <v>65.09999999999999</v>
+        <v>70.80259014109356</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>211.4708162758621</v>
+      </c>
+      <c r="J23" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="24">
@@ -1141,10 +1212,13 @@
         <v>0.578</v>
       </c>
       <c r="H24" t="n">
-        <v>65.09999999999999</v>
+        <v>70.80259014109356</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>235.9211626329114</v>
+      </c>
+      <c r="J24" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -1170,10 +1244,13 @@
         <v>0.7</v>
       </c>
       <c r="H25" t="n">
-        <v>65.09999999999999</v>
+        <v>70.80259014109356</v>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>238.9125260491401</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1199,10 +1276,13 @@
         <v>0.407</v>
       </c>
       <c r="H26" t="n">
-        <v>65.09999999999999</v>
+        <v>70.80259014109356</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>252.8184900585962</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1228,10 +1308,13 @@
         <v>0.227</v>
       </c>
       <c r="H27" t="n">
-        <v>65.09999999999999</v>
+        <v>70.80259014109356</v>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>240.3466045629732</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1260,7 +1343,10 @@
         <v>75</v>
       </c>
       <c r="I28" t="n">
-        <v>6</v>
+        <v>177.2628692307692</v>
+      </c>
+      <c r="J28" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -1289,7 +1375,10 @@
         <v>124.51</v>
       </c>
       <c r="I29" t="n">
-        <v>5</v>
+        <v>254.1618026273788</v>
+      </c>
+      <c r="J29" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -1318,6 +1407,9 @@
         <v>67</v>
       </c>
       <c r="I30" t="n">
+        <v>128.558256097561</v>
+      </c>
+      <c r="J30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1347,7 +1439,10 @@
         <v>66.8</v>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>176.5183923853211</v>
+      </c>
+      <c r="J31" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -1376,7 +1471,10 @@
         <v>59.8</v>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>178.3039076923077</v>
+      </c>
+      <c r="J32" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -1405,7 +1503,10 @@
         <v>88.7</v>
       </c>
       <c r="I33" t="n">
-        <v>2</v>
+        <v>201.5683957709251</v>
+      </c>
+      <c r="J33" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="34">
@@ -1434,7 +1535,10 @@
         <v>51.9</v>
       </c>
       <c r="I34" t="n">
-        <v>3</v>
+        <v>189.2734051807229</v>
+      </c>
+      <c r="J34" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="35">
@@ -1463,7 +1567,10 @@
         <v>76.2</v>
       </c>
       <c r="I35" t="n">
-        <v>6</v>
+        <v>177.2914351291513</v>
+      </c>
+      <c r="J35" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -1492,7 +1599,10 @@
         <v>79.09999999999999</v>
       </c>
       <c r="I36" t="n">
-        <v>6</v>
+        <v>192.5835129032258</v>
+      </c>
+      <c r="J36" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="37">
@@ -1521,7 +1631,10 @@
         <v>80.45999999999999</v>
       </c>
       <c r="I37" t="n">
-        <v>6</v>
+        <v>127.9173560975609</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1550,7 +1663,10 @@
         <v>32.55</v>
       </c>
       <c r="I38" t="n">
-        <v>7</v>
+        <v>209.8638640776699</v>
+      </c>
+      <c r="J38" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="39">
@@ -1579,7 +1695,10 @@
         <v>42.52</v>
       </c>
       <c r="I39" t="n">
-        <v>3</v>
+        <v>175.2765445444422</v>
+      </c>
+      <c r="J39" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="40">
@@ -1608,7 +1727,10 @@
         <v>30.8648218875985</v>
       </c>
       <c r="I40" t="n">
-        <v>7</v>
+        <v>185.7423717468094</v>
+      </c>
+      <c r="J40" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="41">
@@ -1634,10 +1756,13 @@
         <v>1.09</v>
       </c>
       <c r="H41" t="n">
-        <v>65.09999999999999</v>
+        <v>70.80259014109356</v>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>263.0107908872902</v>
+      </c>
+      <c r="J41" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1666,7 +1791,10 @@
         <v>53</v>
       </c>
       <c r="I42" t="n">
-        <v>3</v>
+        <v>146.1845155080214</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1695,7 +1823,10 @@
         <v>70.87</v>
       </c>
       <c r="I43" t="n">
-        <v>6</v>
+        <v>136.2804266409266</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1724,7 +1855,10 @@
         <v>44.32</v>
       </c>
       <c r="I44" t="n">
-        <v>3</v>
+        <v>231.2406951289398</v>
+      </c>
+      <c r="J44" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1753,7 +1887,10 @@
         <v>45.97</v>
       </c>
       <c r="I45" t="n">
-        <v>3</v>
+        <v>160.7258966005666</v>
+      </c>
+      <c r="J45" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="46">
@@ -1782,6 +1919,9 @@
         <v>61.8</v>
       </c>
       <c r="I46" t="n">
+        <v>126.7963636363637</v>
+      </c>
+      <c r="J46" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1811,7 +1951,10 @@
         <v>320</v>
       </c>
       <c r="I47" t="n">
-        <v>1</v>
+        <v>222.8859755102041</v>
+      </c>
+      <c r="J47" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="48">
@@ -1840,6 +1983,9 @@
         <v>69.8</v>
       </c>
       <c r="I48" t="n">
+        <v>133.6775954198473</v>
+      </c>
+      <c r="J48" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1869,7 +2015,10 @@
         <v>65.12</v>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>190.6038227205312</v>
+      </c>
+      <c r="J49" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="50">
@@ -1898,7 +2047,10 @@
         <v>80.251</v>
       </c>
       <c r="I50" t="n">
-        <v>6</v>
+        <v>218.349211721007</v>
+      </c>
+      <c r="J50" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="51">
@@ -1927,7 +2079,10 @@
         <v>59.9467</v>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>154.9662354727303</v>
+      </c>
+      <c r="J51" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="52">
@@ -1956,7 +2111,10 @@
         <v>60.7533</v>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>171.7672587813467</v>
+      </c>
+      <c r="J52" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="53">
@@ -1985,7 +2143,10 @@
         <v>62.14</v>
       </c>
       <c r="I53" t="n">
-        <v>0</v>
+        <v>214.7173207171314</v>
+      </c>
+      <c r="J53" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="54">
@@ -2014,7 +2175,10 @@
         <v>73</v>
       </c>
       <c r="I54" t="n">
-        <v>6</v>
+        <v>213.0718284518829</v>
+      </c>
+      <c r="J54" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="55">
@@ -2043,7 +2207,10 @@
         <v>66</v>
       </c>
       <c r="I55" t="n">
-        <v>0</v>
+        <v>203.8279584659913</v>
+      </c>
+      <c r="J55" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="56">
@@ -2072,7 +2239,10 @@
         <v>80.73</v>
       </c>
       <c r="I56" t="n">
-        <v>6</v>
+        <v>231.2100940170941</v>
+      </c>
+      <c r="J56" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -2101,7 +2271,10 @@
         <v>73</v>
       </c>
       <c r="I57" t="n">
-        <v>6</v>
+        <v>128.697895522388</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -2130,7 +2303,10 @@
         <v>76.2</v>
       </c>
       <c r="I58" t="n">
-        <v>6</v>
+        <v>186.3168966442953</v>
+      </c>
+      <c r="J58" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="59">
@@ -2159,7 +2335,10 @@
         <v>23.24</v>
       </c>
       <c r="I59" t="n">
-        <v>7</v>
+        <v>209.0480375</v>
+      </c>
+      <c r="J59" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="60">
@@ -2188,7 +2367,10 @@
         <v>40.86</v>
       </c>
       <c r="I60" t="n">
-        <v>3</v>
+        <v>192.7620289855073</v>
+      </c>
+      <c r="J60" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="61">
@@ -2217,7 +2399,10 @@
         <v>67</v>
       </c>
       <c r="I61" t="n">
-        <v>0</v>
+        <v>163.9894539682539</v>
+      </c>
+      <c r="J61" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="62">
@@ -2246,6 +2431,9 @@
         <v>94</v>
       </c>
       <c r="I62" t="n">
+        <v>163.628891902834</v>
+      </c>
+      <c r="J62" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2275,7 +2463,10 @@
         <v>82</v>
       </c>
       <c r="I63" t="n">
-        <v>6</v>
+        <v>138.8930606060606</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -2304,6 +2495,9 @@
         <v>87.09999999999999</v>
       </c>
       <c r="I64" t="n">
+        <v>160.282187826087</v>
+      </c>
+      <c r="J64" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2333,7 +2527,10 @@
         <v>29.743871445037</v>
       </c>
       <c r="I65" t="n">
-        <v>7</v>
+        <v>201.7597771771772</v>
+      </c>
+      <c r="J65" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="66">
@@ -2362,7 +2559,10 @@
         <v>47.4</v>
       </c>
       <c r="I66" t="n">
-        <v>3</v>
+        <v>197.6402116719243</v>
+      </c>
+      <c r="J66" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="67">
@@ -2391,7 +2591,10 @@
         <v>26.9</v>
       </c>
       <c r="I67" t="n">
-        <v>7</v>
+        <v>180.1954190476191</v>
+      </c>
+      <c r="J67" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="68">
@@ -2420,7 +2623,10 @@
         <v>42</v>
       </c>
       <c r="I68" t="n">
-        <v>3</v>
+        <v>192.1763793103448</v>
+      </c>
+      <c r="J68" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="69">
@@ -2449,7 +2655,10 @@
         <v>37.8</v>
       </c>
       <c r="I69" t="n">
-        <v>3</v>
+        <v>192.8701104089219</v>
+      </c>
+      <c r="J69" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="70">
@@ -2478,7 +2687,10 @@
         <v>65.2</v>
       </c>
       <c r="I70" t="n">
-        <v>0</v>
+        <v>181.8563975903615</v>
+      </c>
+      <c r="J70" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -2507,7 +2719,10 @@
         <v>66.2</v>
       </c>
       <c r="I71" t="n">
-        <v>0</v>
+        <v>152.7280308823529</v>
+      </c>
+      <c r="J71" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="72">
@@ -2536,6 +2751,9 @@
         <v>95</v>
       </c>
       <c r="I72" t="n">
+        <v>164.3664111888112</v>
+      </c>
+      <c r="J72" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2565,7 +2783,10 @@
         <v>81</v>
       </c>
       <c r="I73" t="n">
-        <v>6</v>
+        <v>170.1288148936171</v>
+      </c>
+      <c r="J73" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="74">
@@ -2594,6 +2815,9 @@
         <v>61.6</v>
       </c>
       <c r="I74" t="n">
+        <v>134.0391735294118</v>
+      </c>
+      <c r="J74" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2623,6 +2847,9 @@
         <v>68</v>
       </c>
       <c r="I75" t="n">
+        <v>132.2711643835617</v>
+      </c>
+      <c r="J75" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2652,7 +2879,10 @@
         <v>112.6575</v>
       </c>
       <c r="I76" t="n">
-        <v>5</v>
+        <v>128.5266777671411</v>
+      </c>
+      <c r="J76" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="77">
@@ -2681,6 +2911,9 @@
         <v>63.7</v>
       </c>
       <c r="I77" t="n">
+        <v>138.5517161490683</v>
+      </c>
+      <c r="J77" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2710,6 +2943,9 @@
         <v>69.41200000000001</v>
       </c>
       <c r="I78" t="n">
+        <v>122.0903581585345</v>
+      </c>
+      <c r="J78" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2739,7 +2975,10 @@
         <v>46.442</v>
       </c>
       <c r="I79" t="n">
-        <v>3</v>
+        <v>157.1136561361632</v>
+      </c>
+      <c r="J79" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="80">
@@ -2768,7 +3007,10 @@
         <v>80.2</v>
       </c>
       <c r="I80" t="n">
-        <v>6</v>
+        <v>119.9004795366795</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -2797,7 +3039,10 @@
         <v>57.32</v>
       </c>
       <c r="I81" t="n">
-        <v>0</v>
+        <v>178.7356301587301</v>
+      </c>
+      <c r="J81" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="82">
@@ -2826,7 +3071,10 @@
         <v>62.91</v>
       </c>
       <c r="I82" t="n">
-        <v>0</v>
+        <v>188.2333185185186</v>
+      </c>
+      <c r="J82" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="83">
@@ -2855,6 +3103,9 @@
         <v>63.5</v>
       </c>
       <c r="I83" t="n">
+        <v>147.2500602006689</v>
+      </c>
+      <c r="J83" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2884,7 +3135,10 @@
         <v>57.2</v>
       </c>
       <c r="I84" t="n">
-        <v>0</v>
+        <v>166.6356631578947</v>
+      </c>
+      <c r="J84" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="85">
@@ -2913,6 +3167,9 @@
         <v>58.1</v>
       </c>
       <c r="I85" t="n">
+        <v>117.8769655172414</v>
+      </c>
+      <c r="J85" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2942,7 +3199,10 @@
         <v>88.17</v>
       </c>
       <c r="I86" t="n">
-        <v>2</v>
+        <v>260.0274157654389</v>
+      </c>
+      <c r="J86" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -2971,7 +3231,10 @@
         <v>73.59999999999999</v>
       </c>
       <c r="I87" t="n">
-        <v>6</v>
+        <v>118.1651999275037</v>
+      </c>
+      <c r="J87" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -3000,7 +3263,10 @@
         <v>75.61468216999999</v>
       </c>
       <c r="I88" t="n">
-        <v>6</v>
+        <v>122.8026928210982</v>
+      </c>
+      <c r="J88" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -3029,7 +3295,10 @@
         <v>108.82</v>
       </c>
       <c r="I89" t="n">
-        <v>5</v>
+        <v>113.134430395489</v>
+      </c>
+      <c r="J89" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="90">
@@ -3058,7 +3327,10 @@
         <v>42.995</v>
       </c>
       <c r="I90" t="n">
-        <v>3</v>
+        <v>255.9015213004625</v>
+      </c>
+      <c r="J90" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -3087,7 +3359,10 @@
         <v>66.01000000000001</v>
       </c>
       <c r="I91" t="n">
-        <v>0</v>
+        <v>165.406010301293</v>
+      </c>
+      <c r="J91" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="92">
@@ -3116,7 +3391,10 @@
         <v>66.95</v>
       </c>
       <c r="I92" t="n">
-        <v>0</v>
+        <v>168.693351334644</v>
+      </c>
+      <c r="J92" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="93">
@@ -3145,7 +3423,10 @@
         <v>110.545</v>
       </c>
       <c r="I93" t="n">
-        <v>5</v>
+        <v>176.6202822889133</v>
+      </c>
+      <c r="J93" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="94">
@@ -3174,7 +3455,10 @@
         <v>65.3</v>
       </c>
       <c r="I94" t="n">
-        <v>0</v>
+        <v>155.2334911659352</v>
+      </c>
+      <c r="J94" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="95">
@@ -3203,7 +3487,10 @@
         <v>74.9687411</v>
       </c>
       <c r="I95" t="n">
-        <v>6</v>
+        <v>255.8861823529412</v>
+      </c>
+      <c r="J95" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -3232,6 +3519,9 @@
         <v>64.33199063000001</v>
       </c>
       <c r="I96" t="n">
+        <v>141.3051496240602</v>
+      </c>
+      <c r="J96" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3261,7 +3551,10 @@
         <v>65.09999999999999</v>
       </c>
       <c r="I97" t="n">
-        <v>0</v>
+        <v>235.819891005291</v>
+      </c>
+      <c r="J97" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -3290,7 +3583,10 @@
         <v>86.88</v>
       </c>
       <c r="I98" t="n">
-        <v>2</v>
+        <v>255.2607464459498</v>
+      </c>
+      <c r="J98" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -3319,7 +3615,10 @@
         <v>49.19</v>
       </c>
       <c r="I99" t="n">
-        <v>3</v>
+        <v>135.3959147324642</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -3348,6 +3647,9 @@
         <v>84.64422052</v>
       </c>
       <c r="I100" t="n">
+        <v>178.9731962131889</v>
+      </c>
+      <c r="J100" t="n">
         <v>2</v>
       </c>
     </row>
@@ -3377,7 +3679,10 @@
         <v>65.09999999999999</v>
       </c>
       <c r="I101" t="n">
-        <v>0</v>
+        <v>168.0001698795181</v>
+      </c>
+      <c r="J101" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="102">
@@ -3406,7 +3711,10 @@
         <v>120</v>
       </c>
       <c r="I102" t="n">
-        <v>5</v>
+        <v>123.86365</v>
+      </c>
+      <c r="J102" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="103">
@@ -3435,7 +3743,10 @@
         <v>73.2</v>
       </c>
       <c r="I103" t="n">
-        <v>6</v>
+        <v>233.793043454039</v>
+      </c>
+      <c r="J103" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -3464,7 +3775,10 @@
         <v>52.2</v>
       </c>
       <c r="I104" t="n">
-        <v>3</v>
+        <v>136.2215</v>
+      </c>
+      <c r="J104" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="105">
@@ -3493,7 +3807,10 @@
         <v>118</v>
       </c>
       <c r="I105" t="n">
-        <v>5</v>
+        <v>248.2423</v>
+      </c>
+      <c r="J105" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="106">
@@ -3522,7 +3839,10 @@
         <v>49</v>
       </c>
       <c r="I106" t="n">
-        <v>3</v>
+        <v>230.2159946902655</v>
+      </c>
+      <c r="J106" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -3551,7 +3871,10 @@
         <v>70.2</v>
       </c>
       <c r="I107" t="n">
-        <v>0</v>
+        <v>157.2081818181818</v>
+      </c>
+      <c r="J107" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="108">
@@ -3580,7 +3903,10 @@
         <v>68.7</v>
       </c>
       <c r="I108" t="n">
-        <v>0</v>
+        <v>266.0761746031746</v>
+      </c>
+      <c r="J108" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -3609,7 +3935,10 @@
         <v>63</v>
       </c>
       <c r="I109" t="n">
-        <v>0</v>
+        <v>211.7785130434783</v>
+      </c>
+      <c r="J109" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="110">
@@ -3638,6 +3967,9 @@
         <v>62.64</v>
       </c>
       <c r="I110" t="n">
+        <v>134.6594236641221</v>
+      </c>
+      <c r="J110" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>